<commit_message>
Update and adding more documents
</commit_message>
<xml_diff>
--- a/Meetings_Supervisor(Recorded).xlsx
+++ b/Meetings_Supervisor(Recorded).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mandev/Desktop/FindAPlayer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E41F3E-E4B1-CB46-A120-B5E94D07F740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A48F861-CF80-6342-8264-DD8F6030A46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3472F906-E43F-FF49-B626-EC2E6F7BA1C2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{3472F906-E43F-FF49-B626-EC2E6F7BA1C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Meeting Dates</t>
   </si>
@@ -135,6 +135,48 @@
   </si>
   <si>
     <t>What is my project about ?</t>
+  </si>
+  <si>
+    <t>23rd May</t>
+  </si>
+  <si>
+    <t>Projecrt Handover with Alex and Charles</t>
+  </si>
+  <si>
+    <t>30th May</t>
+  </si>
+  <si>
+    <t>Demonstration and Feedback on the project</t>
+  </si>
+  <si>
+    <t>Steps on what to do next</t>
+  </si>
+  <si>
+    <t>Interactive maps - needs more work</t>
+  </si>
+  <si>
+    <t>14th June</t>
+  </si>
+  <si>
+    <t>More demonstration on the project</t>
+  </si>
+  <si>
+    <t>Creating an event and saving the information onto a chosen database tool</t>
+  </si>
+  <si>
+    <t>Start writing more on the report</t>
+  </si>
+  <si>
+    <t>22nd June</t>
+  </si>
+  <si>
+    <t>Rough feedback on the report</t>
+  </si>
+  <si>
+    <t>26th June</t>
+  </si>
+  <si>
+    <t>Steps to take before the submission of the projecr</t>
   </si>
 </sst>
 </file>
@@ -166,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -290,32 +332,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -359,6 +375,78 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -367,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -380,10 +468,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01D93AE-9CA2-F545-B452-3226BAAAA716}">
-  <dimension ref="B1:C33"/>
+  <dimension ref="B1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,22 +804,22 @@
   <sheetData>
     <row r="1" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
-      <c r="C3" s="12"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -899,10 +991,94 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="C33" s="7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="14"/>
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="14"/>
+      <c r="C36" s="10"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="14"/>
+      <c r="C38" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39" s="17"/>
+      <c r="C39" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40" s="14"/>
+      <c r="C40" s="10"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42" s="14"/>
+      <c r="C42" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43" s="17"/>
+      <c r="C43" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="14"/>
+      <c r="C44" s="10"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46" s="14"/>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="2:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>